<commit_message>
Update POS system to v1.0MD with source tracking and damaged inventory
- Implemented product source management (Delivery Receipt, Remaining, Transfers, Beverages).
- Updated products.xlsx loading to support new source columns and DR Price.
- Added 'TA' (Damaged Inventory) tab with Damaged In, Returns, and Flush functions.
- Implemented automatic daily rollover of stock from DR/Transfers to Remaining.
- Updated sales logic to deplete stock from sources in specified order.
- Updated reporting to show DR Total and Damaged quantities.
- Updated PDF generation to group items by Source.
- Added `damagereceipts` folder for damaged inventory receipts.
</commit_message>
<xml_diff>
--- a/products.xlsx
+++ b/products.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,6 +454,31 @@
           <t>Price</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Src_DeliveryReceipt</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Src_Remaining</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Src_Transfers</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Src_Beverages</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>DR Price</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -473,6 +498,21 @@
       </c>
       <c r="D2" t="n">
         <v>100</v>
+      </c>
+      <c r="E2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>